<commit_message>
updated protected templates and added file structure for expansion and rehabilitation
</commit_message>
<xml_diff>
--- a/src/templates/Cocoon_Template.xlsx
+++ b/src/templates/Cocoon_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devvi\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54B2091D-B19F-459F-9ADA-BABE673C3647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF43600-EA30-4240-A242-B58909B19FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -276,10 +276,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="12" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -291,15 +287,15 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -307,8 +303,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="12" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -538,7 +535,7 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -559,16 +556,16 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
       <c r="L1" s="7"/>
       <c r="M1" s="1"/>
     </row>
@@ -576,16 +573,16 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
       <c r="L2" s="7"/>
       <c r="M2" s="1"/>
     </row>
@@ -593,16 +590,16 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
       <c r="L3" s="7"/>
       <c r="M3" s="1"/>
     </row>
@@ -612,14 +609,14 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
       <c r="L4" s="7"/>
       <c r="M4" s="1"/>
     </row>
@@ -627,28 +624,28 @@
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="6" t="s">
@@ -667,13 +664,13 @@
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -686,25 +683,25 @@
       <c r="B7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="14" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="5">
@@ -721,184 +718,184 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="13"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="14"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="13"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="12"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="14"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="13"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="14"/>
+      <c r="M10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="13"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="14"/>
+      <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="13"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="14"/>
+      <c r="M12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="13"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="14"/>
+      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="13"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="14"/>
+      <c r="M14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="13"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="14"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="13"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="12"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="14"/>
+      <c r="M16" s="13"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="13"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="14"/>
+      <c r="M17" s="13"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="13"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="12"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="14"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="13"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="14"/>
+      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1261,7 +1258,7 @@
       <c r="M43" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WdsiJF7q+w2z4uL4rrrOgUz1d9cTNRMqds3q0DI60JecmPYYoom1SmHWiNgbCGOrFkzDQwo+qHHtKrTnRc9C7g==" saltValue="zauDhGJmWwCCqvFZuYsyCg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="D2:K2"/>

</xml_diff>

<commit_message>
changed logic for graph, fixed distri, nursery, templates, config, schema.
</commit_message>
<xml_diff>
--- a/src/templates/Cocoon_Template.xlsx
+++ b/src/templates/Cocoon_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devvi\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF43600-EA30-4240-A242-B58909B19FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9834A4ED-309A-4D26-B57D-EA572B01B1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1191" yWindow="3429" windowWidth="31723" windowHeight="14365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Regional Office _____________</t>
   </si>
   <si>
-    <t>Regional Office 4</t>
-  </si>
-  <si>
     <t>Oriental Mindoro</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Cocoon Production Upload Form</t>
+  </si>
+  <si>
+    <t>Region 4</t>
   </si>
 </sst>
 </file>
@@ -535,24 +535,24 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.84375" style="2" customWidth="1"/>
     <col min="3" max="6" width="20" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.84375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.69140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="15" style="2" customWidth="1"/>
     <col min="10" max="10" width="20" style="2" customWidth="1"/>
-    <col min="11" max="12" width="20.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="12.5703125" style="2"/>
+    <col min="11" max="12" width="20.53515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="25.53515625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="12.53515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -569,7 +569,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -586,7 +586,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -603,9 +603,9 @@
       <c r="L3" s="7"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="1"/>
@@ -620,12 +620,12 @@
       <c r="L4" s="7"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>0</v>
@@ -643,25 +643,25 @@
         <v>3</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="J5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="15"/>
@@ -676,33 +676,33 @@
       <c r="L6" s="4"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A7" s="9">
         <v>44553</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="14" t="s">
         <v>22</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="J7" s="5">
         <v>3000</v>
@@ -717,7 +717,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="16"/>
@@ -732,7 +732,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
@@ -747,7 +747,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="16"/>
@@ -762,7 +762,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="16"/>
@@ -777,7 +777,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16"/>
@@ -792,7 +792,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="16"/>
@@ -807,7 +807,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
@@ -822,7 +822,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
@@ -837,7 +837,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="13"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="16"/>
@@ -852,7 +852,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="16"/>
@@ -867,7 +867,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="13"/>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="16"/>
@@ -882,7 +882,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="13"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="16"/>
@@ -897,7 +897,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="13"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -912,7 +912,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -927,7 +927,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -942,7 +942,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -957,7 +957,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -972,7 +972,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -987,7 +987,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1002,7 +1002,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1017,7 +1017,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1032,7 +1032,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1047,7 +1047,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1062,7 +1062,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1077,7 +1077,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1092,7 +1092,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1107,7 +1107,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1122,7 +1122,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1137,7 +1137,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1152,7 +1152,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1167,7 +1167,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1182,7 +1182,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1197,7 +1197,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1212,7 +1212,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1227,7 +1227,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1242,7 +1242,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>

</xml_diff>

<commit_message>
updated materials, cocoon and expansion modules
</commit_message>
<xml_diff>
--- a/src/templates/Cocoon_Template.xlsx
+++ b/src/templates/Cocoon_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasta\OneDrive\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7B94A6D-416A-4F21-BBEC-541147F63187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{674BC2FF-D47C-4D6B-A637-0C2AB2E3D74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Region</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Regional Office 4</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -289,6 +292,10 @@
     </xf>
     <xf numFmtId="12" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="12" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -516,10 +523,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -532,11 +539,11 @@
     <col min="11" max="11" width="15" style="2" customWidth="1"/>
     <col min="12" max="12" width="20" style="2" customWidth="1"/>
     <col min="13" max="14" width="20.5703125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="25.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="12.5703125" style="2"/>
+    <col min="15" max="16" width="25.5703125" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -554,8 +561,9 @@
       <c r="M1" s="14"/>
       <c r="N1" s="6"/>
       <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -573,8 +581,9 @@
       <c r="M2" s="14"/>
       <c r="N2" s="6"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -592,8 +601,9 @@
       <c r="M3" s="14"/>
       <c r="N3" s="6"/>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
@@ -611,8 +621,9 @@
       <c r="M4" s="14"/>
       <c r="N4" s="6"/>
       <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -658,8 +669,11 @@
       <c r="O5" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P5" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="10"/>
@@ -675,8 +689,9 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>44553</v>
       </c>
@@ -722,8 +737,9 @@
       <c r="O7" s="13">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -739,8 +755,9 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -756,8 +773,9 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -773,8 +791,9 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -790,8 +809,9 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -807,8 +827,9 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -824,8 +845,9 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -841,8 +863,9 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -858,8 +881,9 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -875,8 +899,9 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -892,8 +917,9 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -909,8 +935,9 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -926,8 +953,9 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -943,8 +971,9 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -960,8 +989,9 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -977,8 +1007,9 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -994,8 +1025,9 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1011,8 +1043,9 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1028,8 +1061,9 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1045,8 +1079,9 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1062,8 +1097,9 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1079,8 +1115,9 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1096,8 +1133,9 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1113,8 +1151,9 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1130,8 +1169,9 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1147,8 +1187,9 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1164,8 +1205,9 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1181,8 +1223,9 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1198,8 +1241,9 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1215,8 +1259,9 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1232,8 +1277,9 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-    </row>
-    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1249,8 +1295,9 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1266,8 +1313,9 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-    </row>
-    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1283,8 +1331,9 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-    </row>
-    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P40" s="3"/>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1300,8 +1349,9 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-    </row>
-    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P41" s="3"/>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1317,8 +1367,9 @@
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
-    </row>
-    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1334,6 +1385,7 @@
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="vws1z1OO7JirILgvP8vCuTiHU6DSJR4DjG8UuNlRJBCKFx/Cz2VqOtZ+nJczvyk9jBSoXeEh+S1YmAFAKCNuLg==" saltValue="ciItJRzr863FMQQrcvCAdQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>